<commit_message>
Removido consulta CcsXi. Documentação. Limpeza de codigo. Ajustes finos finais.
</commit_message>
<xml_diff>
--- a/Documentacao/Migração PI-PO Descrição dos fontes Java e Tecnologias Utilizadas.xlsx
+++ b/Documentacao/Migração PI-PO Descrição dos fontes Java e Tecnologias Utilizadas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
   <si>
     <t>Código</t>
   </si>
@@ -226,15 +226,6 @@
     <t>z-provisionamento-all</t>
   </si>
   <si>
-    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco de Dados. Api JaxB para fazer o mapeamento de Xml para Objeto Java.</t>
-  </si>
-  <si>
-    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco de Dados.</t>
-  </si>
-  <si>
-    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco de Dados. JCO para acesso a funções remotas.</t>
-  </si>
-  <si>
     <t>z-memoria-massa</t>
   </si>
   <si>
@@ -254,6 +245,18 @@
   </si>
   <si>
     <t>Pacote Java gerado</t>
+  </si>
+  <si>
+    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco remoto de Dados. Api JaxB para fazer o mapeamento de Xml para Objeto Java.</t>
+  </si>
+  <si>
+    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco remoto de Dados.</t>
+  </si>
+  <si>
+    <t>Java Dom (W3C) para manipular nodes e Xml Transform para renderizar conteudo. Componente Ejb 3.0 para acesso ao Banco remoto de Dados. JCO para acesso a funções remotas.</t>
+  </si>
+  <si>
+    <t>Promove a manipulação padrão de nodes xml, buscando uma data pré definida e atribuindo seu valor aos nodes marcados como pendentes de de atualização.</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1287,7 @@
   <dimension ref="A1:D327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1297,16 +1300,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,7 +1393,7 @@
         <v>52</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,7 +1407,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1418,7 +1421,7 @@
         <v>54</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1432,7 +1435,7 @@
         <v>54</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1446,7 +1449,7 @@
         <v>54</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,22 +1460,24 @@
         <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>